<commit_message>
Modifying the Code making the users understand what I am doing
</commit_message>
<xml_diff>
--- a/Automating Excel Sheet.xlsx
+++ b/Automating Excel Sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DataScience\Machine-Learning-Projects\Automate Google Forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DataScience\Machine-Learning-Projects\Automate Google Forms\Autofill-Google-Forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41D1CA0-6869-4CFD-93F8-B47813C3B6D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581AD334-A9EB-4386-87A0-FBC057D1E9FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{ADBBC5D6-AA3B-4F44-9A48-84D9CF62FCEE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Page No.</t>
   </si>
@@ -76,24 +76,6 @@
   </si>
   <si>
     <t>Final Link</t>
-  </si>
-  <si>
-    <t>emailAddress="noname7231236@gmail.com</t>
-  </si>
-  <si>
-    <t>entry.1585933220="9912546853</t>
-  </si>
-  <si>
-    <t>entry.1534863658="Yes</t>
-  </si>
-  <si>
-    <t>entry.1274209221="Mobile</t>
-  </si>
-  <si>
-    <t>entry.759405699="VR</t>
-  </si>
-  <si>
-    <t>entry.767675694="SOME</t>
   </si>
 </sst>
 </file>
@@ -465,22 +447,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B655E37-ACC0-47AE-9A12-C445B3999E5F}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="31.44140625" customWidth="1"/>
-    <col min="3" max="3" width="131" customWidth="1"/>
-    <col min="4" max="4" width="69.109375" customWidth="1"/>
-    <col min="5" max="5" width="59.33203125" customWidth="1"/>
-    <col min="6" max="6" width="51.5546875" customWidth="1"/>
-    <col min="7" max="7" width="56.33203125" customWidth="1"/>
-    <col min="8" max="8" width="49.6640625" customWidth="1"/>
-    <col min="9" max="9" width="53.88671875" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.21875" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" customWidth="1"/>
+    <col min="9" max="9" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -540,26 +523,6 @@
       </c>
       <c r="I2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>